<commit_message>
Updated test execution results
</commit_message>
<xml_diff>
--- a/OpenCart-ManualTesting-main/Bug Report(OpenCart).xlsx
+++ b/OpenCart-ManualTesting-main/Bug Report(OpenCart).xlsx
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>Warning message with the text ' Warning: Your account has exceeded allowed number of login attempts. Please try again in 1 hour.' should be displayed for the 5th time of clicking the 'Login' button with the same invalid credentials</t>
-  </si>
-  <si>
-    <t>No any warning message displayed on continous linvalid login attempts for for than 5 times</t>
   </si>
   <si>
     <t>OPEN_CART_BUG_8</t>
@@ -458,16 +455,26 @@
 2. Click on 'Add to Cart' icon option in the displayed 'My Wish List' page 
 3. Click on 'Shopping Cart' header option </t>
   </si>
+  <si>
+    <t>No any warning message displayed on continous linvalid login attempts for more than 5 times</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -610,75 +617,78 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,8 +910,8 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -968,7 +978,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
@@ -1094,7 +1104,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>28</v>
@@ -1225,8 +1235,8 @@
       <c r="D8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>45</v>
+      <c r="E8" s="25" t="s">
+        <v>111</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>12</v>
@@ -1256,19 +1266,19 @@
     </row>
     <row r="9" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="D9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>12</v>
@@ -1298,25 +1308,25 @@
     </row>
     <row r="10" spans="1:26" ht="263.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>35</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
@@ -1340,19 +1350,19 @@
     </row>
     <row r="11" spans="1:26" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>19</v>
@@ -1382,19 +1392,19 @@
     </row>
     <row r="12" spans="1:26" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="D12" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>19</v>
@@ -1424,19 +1434,19 @@
     </row>
     <row r="13" spans="1:26" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>19</v>
@@ -1466,19 +1476,19 @@
     </row>
     <row r="14" spans="1:26" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>19</v>
@@ -1508,19 +1518,19 @@
     </row>
     <row r="15" spans="1:26" ht="173.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>19</v>
@@ -1550,19 +1560,19 @@
     </row>
     <row r="16" spans="1:26" ht="219.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>19</v>
@@ -1592,19 +1602,19 @@
     </row>
     <row r="17" spans="1:26" ht="205" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>84</v>
-      </c>
       <c r="C17" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>19</v>
@@ -1634,19 +1644,19 @@
     </row>
     <row r="18" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="D18" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>12</v>
@@ -1676,19 +1686,19 @@
     </row>
     <row r="19" spans="1:26" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>93</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>19</v>
@@ -1718,19 +1728,19 @@
     </row>
     <row r="20" spans="1:26" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="E20" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>19</v>
@@ -1760,25 +1770,25 @@
     </row>
     <row r="21" spans="1:26" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>102</v>
-      </c>
       <c r="G21" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="1"/>

</xml_diff>